<commit_message>
20260111_newest simulation model & data & result & readme
</commit_message>
<xml_diff>
--- a/outputs/simulation_configs/simulation_parameters.xlsx
+++ b/outputs/simulation_configs/simulation_parameters.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Efficiency" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Production_Rate" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Buffer_Capacity" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Hourly_Arrivals" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Hourly_Arrivals" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -574,79 +573,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Required Trailers</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Trailers</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Accumulated Pallets (6hr)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>R&amp;P</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
-        <v>123.6590909090909</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FG</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>253.0440729483283</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
new logic, new data
</commit_message>
<xml_diff>
--- a/outputs/simulation_configs/simulation_parameters.xlsx
+++ b/outputs/simulation_configs/simulation_parameters.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Efficiency" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Production_Rate" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Hourly_Arrivals" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Efficiency" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Production_Rate" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hourly_Arrivals" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
feat: Add dynamic scheduling demonstration and architecture documentation
- Implemented a new script `demo_dynamic_scheduling.py` to showcase dynamic priority queue scheduling for outbound orders.
- Created architecture descriptions in `ARCHITECTURE_DESCRIPTIONS.md` detailing the overall architecture, outbound and inbound processes.
- Added a 2-minute presentation script in `PRESENTATION_SCRIPT_2MIN.md` for effective communication of the simulation model.
- Developed a comprehensive overview of the simulation architecture in `SIMULATION_ARCHITECTURE_BRIEF.md`.
- Introduced unit tests in `test_priority_queue.py` to validate the core logic of the priority queue scheduling.
</commit_message>
<xml_diff>
--- a/outputs/simulation_configs/simulation_parameters.xlsx
+++ b/outputs/simulation_configs/simulation_parameters.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Efficiency" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Production_Rate" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hourly_Arrivals" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Efficiency" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Production_Rate" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Hourly_Arrivals" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Refactor KPICollector and DCSimulation classes; remove deprecated test_priority_queue.py
- Cleaned up KPICollector by removing unnecessary comments and improving code clarity.
- Simplified the record_dock_usage and record_inbound_delay methods.
- Updated DCSimulation initialization to enhance readability and maintainability.
- Removed the test_priority_queue.py file as it was no longer needed.
</commit_message>
<xml_diff>
--- a/outputs/simulation_configs/simulation_parameters.xlsx
+++ b/outputs/simulation_configs/simulation_parameters.xlsx
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.60984848484848</v>
+        <v>20.25889121338912</v>
       </c>
       <c r="C2" t="n">
-        <v>494.6363636363636</v>
+        <v>486.2133891213389</v>
       </c>
     </row>
     <row r="3">
@@ -556,10 +556,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42.17401215805472</v>
+        <v>42.29901960784314</v>
       </c>
       <c r="C3" t="n">
-        <v>1012.176291793313</v>
+        <v>1015.176470588235</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.003278688524590164</v>
+        <v>0.004184100418410041</v>
       </c>
     </row>
     <row r="3">
@@ -606,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003278688524590164</v>
+        <v>0.004184100418410041</v>
       </c>
     </row>
     <row r="4">
@@ -614,7 +614,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>2.383606557377049</v>
+        <v>2.456066945606695</v>
       </c>
     </row>
     <row r="5">
@@ -622,7 +622,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>3.931147540983607</v>
+        <v>4.138075313807532</v>
       </c>
     </row>
     <row r="6">
@@ -630,7 +630,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>3.60327868852459</v>
+        <v>3.740585774058578</v>
       </c>
     </row>
     <row r="7">
@@ -638,7 +638,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>3.744262295081967</v>
+        <v>3.912133891213389</v>
       </c>
     </row>
     <row r="8">
@@ -646,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>4.114754098360656</v>
+        <v>4.133891213389122</v>
       </c>
     </row>
     <row r="9">
@@ -654,7 +654,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>4.288524590163934</v>
+        <v>4.221757322175733</v>
       </c>
     </row>
     <row r="10">
@@ -662,7 +662,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>3.937704918032787</v>
+        <v>3.94142259414226</v>
       </c>
     </row>
     <row r="11">
@@ -670,7 +670,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>3.839344262295082</v>
+        <v>3.841004184100418</v>
       </c>
     </row>
     <row r="12">
@@ -678,7 +678,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>3.849180327868853</v>
+        <v>3.907949790794979</v>
       </c>
     </row>
     <row r="13">
@@ -686,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>3.583606557377049</v>
+        <v>3.644351464435146</v>
       </c>
     </row>
     <row r="14">
@@ -694,7 +694,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>3.518032786885246</v>
+        <v>3.510460251046025</v>
       </c>
     </row>
     <row r="15">
@@ -702,7 +702,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>2.973770491803279</v>
+        <v>3.01255230125523</v>
       </c>
     </row>
     <row r="16">
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>2.760655737704918</v>
+        <v>2.778242677824268</v>
       </c>
     </row>
     <row r="17">
@@ -718,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>3.01311475409836</v>
+        <v>3.125523012552301</v>
       </c>
     </row>
     <row r="18">
@@ -726,7 +726,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>1.472131147540984</v>
+        <v>1.640167364016736</v>
       </c>
     </row>
     <row r="19">
@@ -734,7 +734,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.9836065573770492</v>
+        <v>1.225941422594142</v>
       </c>
     </row>
     <row r="20">
@@ -742,7 +742,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.6721311475409836</v>
+        <v>0.7949790794979079</v>
       </c>
     </row>
     <row r="21">
@@ -750,7 +750,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.360655737704918</v>
+        <v>0.4476987447698745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>